<commit_message>
* updating power budget spreadsheet
</commit_message>
<xml_diff>
--- a/docs/power_budget.xlsx
+++ b/docs/power_budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel2\projects\copper_suicide\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\projects\copper-suicide\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,6 +23,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>joel</author>
+  </authors>
+  <commentList>
+    <comment ref="AB10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>joel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Includes power from all other rails.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
@@ -195,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +259,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +306,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -425,6 +478,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -705,11 +759,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1239,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="17">
+      <c r="AB10" s="28">
         <v>8.9499999999999993</v>
       </c>
       <c r="AC10" s="16">
@@ -2798,5 +2852,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* lots of schematic cleanup
</commit_message>
<xml_diff>
--- a/docs/power_budget.xlsx
+++ b/docs/power_budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\projects\copper-suicide\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel2\projects\copper_suicide\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>joel:</t>
         </r>
@@ -46,7 +46,7 @@
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Includes power from all other rails.</t>
@@ -263,14 +263,14 @@
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -475,10 +475,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -762,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,29 +777,29 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="23" t="s">
         <v>46</v>
@@ -920,7 +920,7 @@
         <v>0.42</v>
       </c>
       <c r="F7">
-        <v>0.36499999999999999</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -981,11 +981,11 @@
       </c>
       <c r="AA7" s="18">
         <f>SUM(E7:Y7)</f>
-        <v>0.78499999999999992</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="AB7" s="17">
         <f>AA7</f>
-        <v>0.78499999999999992</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="AC7" s="16">
         <v>1.5</v>
@@ -1239,7 +1239,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="28">
+      <c r="AB10" s="27">
         <v>8.9499999999999993</v>
       </c>
       <c r="AC10" s="16">
@@ -1666,29 +1666,29 @@
       </c>
     </row>
     <row r="20" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="28"/>
     </row>
     <row r="21" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E21" s="9" t="str">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="F23" s="4">
         <f t="shared" ref="F23:Y23" si="2">F7*$C7</f>
-        <v>1.2044999999999999</v>
+        <v>1.4684999999999999</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" ref="G23" si="3">G7*$C7</f>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="AA23" s="4">
         <f>SUM(E23:Y23)</f>
-        <v>2.5904999999999996</v>
+        <v>2.8544999999999998</v>
       </c>
       <c r="AB23" t="s">
         <v>53</v>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="F33" s="4">
         <f>SUM(F23:F31)</f>
-        <v>1.2044999999999999</v>
+        <v>1.4684999999999999</v>
       </c>
       <c r="G33" s="4">
         <f>SUM(G23:G31)</f>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="AC33" s="4">
         <f>AA31+AA30+AA29+AA28+AA25+AA24+AA23</f>
-        <v>98.798699999999982</v>
+        <v>99.062699999999978</v>
       </c>
     </row>
     <row r="34" spans="4:29" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="AC35" s="26">
         <f>AC33/AC34</f>
-        <v>107.3898913043478</v>
+        <v>107.67684782608693</v>
       </c>
     </row>
     <row r="37" spans="4:29" x14ac:dyDescent="0.25">

</xml_diff>